<commit_message>
unused attributes were removed
</commit_message>
<xml_diff>
--- a/configs/attributes_delivery_order.xlsx
+++ b/configs/attributes_delivery_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demidov_ai\Documents\Демидов\Питон\appius-mto-neosintez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demid\Documents\python\work_projects\appius-mto-neosintez\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47239E91-20F9-4C79-BC84-F73FC06D20ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBBA645-1E7E-4A4D-8169-383B6A0BAB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACD5EDCE-5462-4D4A-8670-E1A96D14B552}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -48,9 +48,6 @@
     <t>2255f35e-5e60-e911-8115-817c3f53a992</t>
   </si>
   <si>
-    <t>ddb5bdc1-dd8d-e911-8116-dc30078865da</t>
-  </si>
-  <si>
     <t>29c13432-f76f-e911-8115-817c3f53a992</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Документ заказа.Дата завершения комплектации</t>
   </si>
   <si>
-    <t>Документ заказа.Договор контрагента</t>
-  </si>
-  <si>
     <t>Документ заказа.Статус</t>
   </si>
   <si>
@@ -123,18 +117,6 @@
     <t>Доставлено на склад получатель</t>
   </si>
   <si>
-    <t>Документ заказа.Ответственное лицо со стороны подрядчика</t>
-  </si>
-  <si>
-    <t>Документ заказа.Вид расходного документа</t>
-  </si>
-  <si>
-    <t>Документ заказа.Составитель</t>
-  </si>
-  <si>
-    <t>Документ заказа.Комментарий</t>
-  </si>
-  <si>
     <t>626370d8-ad8f-ec11-911d-005056b6948b</t>
   </si>
   <si>
@@ -153,9 +135,6 @@
     <t>c0ae40d6-72fb-ec11-9136-005056b6948b</t>
   </si>
   <si>
-    <t>3e55de1a-15f8-ec11-9134-005056b6948b</t>
-  </si>
-  <si>
     <t>fdde6847-c6cf-ea11-9110-005056b6948b</t>
   </si>
   <si>
@@ -163,15 +142,6 @@
   </si>
   <si>
     <t>6f93288c-6ffb-ec11-9136-005056b6948b</t>
-  </si>
-  <si>
-    <t>24fb608a-2c5d-ea11-910f-005056b6948b</t>
-  </si>
-  <si>
-    <t>af259515-f864-e911-8115-817c3f53a992</t>
-  </si>
-  <si>
-    <t>ab479cfc-f496-e911-80cd-9783b3495d40</t>
   </si>
   <si>
     <t>c60bff0b-8759-ec11-911a-005056b6948b</t>
@@ -205,10 +175,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -235,13 +213,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -257,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -403,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,303 +532,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C59750-CE11-4137-A397-5E625D311B92}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A18" sqref="A18:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>